<commit_message>
Reorganize files in directories
</commit_message>
<xml_diff>
--- a/json_to_ncbi1/test_ncbi_metadata.xlsx
+++ b/json_to_ncbi1/test_ncbi_metadata.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SARS-CoV-2.cl.1.0" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="SARS-CoV-2.cl.1.0" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -707,7 +707,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -3383,21 +3383,21 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation sqref="AD13:AD1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" error="Wrong value, try again." type="list">
+    <dataValidation sqref="AD13:AD1048576" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" error="Wrong value, try again." type="list">
       <formula1>"male,female,pooled male and female,neuter,hermaphrodite,intersex,not determined,missing,not applicable,not collected,not provided,restricted access"</formula1>
     </dataValidation>
-    <dataValidation sqref="AJ13:AK1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" error="Wrong value, try again." type="list">
+    <dataValidation sqref="AJ13:AK1048576" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" error="Wrong value, try again." type="list">
       <formula1>"no,yes"</formula1>
     </dataValidation>
-    <dataValidation sqref="AL13:AL1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" error="Wrong value, try again." type="list">
+    <dataValidation sqref="AL13:AL1048576" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" error="Wrong value, try again." type="list">
       <formula1>"no,yes - completed,yes - partially completed"</formula1>
     </dataValidation>
-    <dataValidation sqref="AO13:AP1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" error="Wrong value, try again." type="list">
+    <dataValidation sqref="AO13:AP1048576" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" error="Wrong value, try again." type="list">
       <formula1>"E (orf4),M (orf5),N (orf9),spike (orf2),ORF1ab (rep),ORF1a (pp1a),nsp11,nsp1,nsp2,nsp3,nsp4,nsp5,nsp6,nsp7,nsp8,nsp9,nsp10,nsp12 (RdRp),nsp13 (Hel),nsp14 (ExoN),nsp15,nsp16,ORF3a,ORF3b,ORF6 (ns6),ORF7a,ORF7b (ns7b),ORF8 (ns8),ORF9b,ORF9c,ORF10,ORF14"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
</xml_diff>